<commit_message>
✏️ Small text fixes
</commit_message>
<xml_diff>
--- a/export/scostamento_prezzo.xlsx
+++ b/export/scostamento_prezzo.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Δ E-TE</t>
+          <t>Δ Tasso di cambio</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -451,7 +451,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Δ TE-C</t>
+          <t>Δ Prezzo</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>